<commit_message>
Extract service validation logic into separate validators and implement controller layer
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agale\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agale\IdeaProjects\invoice-maker-2.0\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6AAEA0-0899-4EC9-9C42-DD0E2666D576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093C5DCA-A5A1-4B1E-A66D-F3396E52D6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17388" yWindow="-5484" windowWidth="17496" windowHeight="30216" xr2:uid="{8D217AB8-E05B-4861-AD59-D31F3C33ECF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{8D217AB8-E05B-4861-AD59-D31F3C33ECF7}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -168,9 +168,6 @@
     <t>{{lesson.summary.remaining}}</t>
   </si>
   <si>
-    <t>{{payedMark}}</t>
-  </si>
-  <si>
     <t>{{invoice.variableSymbol}}</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>Tel.:</t>
+  </si>
+  <si>
+    <t>{{lesson.payedMark}}</t>
   </si>
 </sst>
 </file>
@@ -518,18 +518,105 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -538,93 +625,6 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -943,7 +943,7 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,80 +958,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="45" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="49"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="50"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="51"/>
     </row>
     <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="56"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="49"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="48"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
+      <c r="A4" s="60"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="50"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="27"/>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="39"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="28"/>
       <c r="I5" s="29"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="55"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="27"/>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="39"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="28"/>
       <c r="I6" s="29"/>
     </row>
@@ -1041,10 +1041,10 @@
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="39"/>
+      <c r="G7" s="56"/>
       <c r="H7" s="28"/>
       <c r="I7" s="29"/>
     </row>
@@ -1056,10 +1056,10 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="39"/>
+      <c r="G8" s="56"/>
       <c r="H8" s="28"/>
       <c r="I8" s="29"/>
     </row>
@@ -1071,8 +1071,8 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="28"/>
       <c r="I9" s="29"/>
     </row>
@@ -1087,11 +1087,11 @@
       <c r="F10" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="40"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="69"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
@@ -1102,19 +1102,19 @@
       <c r="F11" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="69"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="14"/>
       <c r="F12" s="9"/>
       <c r="G12" s="28"/>
@@ -1122,12 +1122,12 @@
       <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="14"/>
       <c r="F13" s="9"/>
       <c r="G13" s="28"/>
@@ -1135,14 +1135,14 @@
       <c r="I13" s="29"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="62" t="s">
+      <c r="B14" s="54"/>
+      <c r="C14" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="62"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="8"/>
       <c r="F14" s="11"/>
       <c r="G14" s="28"/>
@@ -1154,8 +1154,8 @@
         <v>10</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="8"/>
       <c r="F15" s="11"/>
       <c r="G15" s="28"/>
@@ -1163,12 +1163,12 @@
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="15"/>
       <c r="F16" s="16"/>
       <c r="G16" s="30"/>
@@ -1180,36 +1180,36 @@
         <v>11</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="34"/>
       <c r="F17" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="60" t="s">
+      <c r="H17" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="61"/>
+      <c r="I17" s="65"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="17"/>
-      <c r="C18" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="57"/>
+      <c r="C18" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="61"/>
       <c r="E18" s="18"/>
       <c r="F18" s="16" t="s">
         <v>25</v>
       </c>
       <c r="G18" s="16"/>
-      <c r="H18" s="68" t="s">
+      <c r="H18" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="69"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1224,12 +1224,12 @@
       <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
@@ -1237,12 +1237,12 @@
       <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -1338,46 +1338,46 @@
       <c r="I29" s="18"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="54"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="44"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G30" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="44" t="s">
+      <c r="H30" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="I30" s="70"/>
+      <c r="I30" s="43"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="67"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="22"/>
-      <c r="D31" s="71" t="s">
+      <c r="D31" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="71"/>
+      <c r="E31" s="45"/>
       <c r="F31" s="31" t="s">
         <v>38</v>
       </c>
       <c r="G31" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="H31" s="41" t="s">
+      <c r="H31" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="42"/>
+      <c r="I31" s="71"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
@@ -1400,10 +1400,10 @@
       <c r="G33" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="I33" s="37"/>
+      <c r="H33" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="I33" s="66"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
@@ -1415,10 +1415,10 @@
       <c r="G34" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H34" s="36" t="s">
+      <c r="H34" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="I34" s="36"/>
+      <c r="I34" s="67"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
@@ -1430,10 +1430,10 @@
       <c r="G35" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H35" s="37" t="s">
+      <c r="H35" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I35" s="37"/>
+      <c r="I35" s="66"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="25"/>
@@ -1452,12 +1452,12 @@
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
-      <c r="F37" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
+      <c r="F37" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="68"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="68"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
@@ -1573,12 +1573,12 @@
       <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="57"/>
+      <c r="C49" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B49" s="43"/>
-      <c r="C49" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="3"/>
@@ -1591,23 +1591,12 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="E3:I4"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="H31:I31"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="F1:G2"/>
@@ -1624,12 +1613,23 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="E3:I4"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="D31:E31"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:D14" xr:uid="{8578971D-8F84-435B-B113-CCAE2785435F}">

</xml_diff>